<commit_message>
Add 04 09 + mt @SvyTo
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/club_akhmat.xlsx
+++ b/RPL_V2/xlsx/club_akhmat.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SvyTo\PycharmProjects\amaranth64.github.io\RPL_V2\xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -186,6 +181,9 @@
     <t>akh_kovachev</t>
   </si>
   <si>
+    <t>akh_samorodov</t>
+  </si>
+  <si>
     <t>5-е место в 2016/17 и 2022/23</t>
   </si>
   <si>
@@ -240,6 +238,9 @@
     <t>26-летний(14.03.1998) болгарский нападающий. Перешёл в Ахмат летом 2024 из болгарской Арды</t>
   </si>
   <si>
+    <t>22-летний(29.06.2002) казахский нападающий. Перешёл в Ахмат летом 2024 из Актобе</t>
+  </si>
+  <si>
     <t>cup_uefa</t>
   </si>
   <si>
@@ -285,192 +286,195 @@
     <t>Виталий Якушкин</t>
   </si>
   <si>
-    <t> Анатолий Синько</t>
+    <t xml:space="preserve"> Анатолий Синько</t>
+  </si>
+  <si>
+    <t>Гамид Агаларов</t>
+  </si>
+  <si>
+    <t>Бернард Бериша</t>
+  </si>
+  <si>
+    <t>Гиорги Шелия</t>
+  </si>
+  <si>
+    <t>Антон Швец</t>
+  </si>
+  <si>
+    <t>Камило</t>
+  </si>
+  <si>
+    <t>Мирослав Богосовац</t>
+  </si>
+  <si>
+    <t>Надер Гандри</t>
+  </si>
+  <si>
+    <t>Лукас Ловат</t>
+  </si>
+  <si>
+    <t>Дарко Тодорович</t>
+  </si>
+  <si>
+    <t>Амин Талал</t>
+  </si>
+  <si>
+    <t>Заим Диванович</t>
+  </si>
+  <si>
+    <t>Милош Шатара</t>
+  </si>
+  <si>
+    <t>Евгений Харин</t>
+  </si>
+  <si>
+    <t>Исмаэл Силва</t>
+  </si>
+  <si>
+    <t>Феллипе Кардозо</t>
+  </si>
+  <si>
+    <t>Мауро Луна</t>
+  </si>
+  <si>
+    <t>Светослав Ковачев</t>
+  </si>
+  <si>
+    <t>Максим Самородов</t>
+  </si>
+  <si>
+    <t>num_6</t>
+  </si>
+  <si>
+    <t>6-е</t>
+  </si>
+  <si>
+    <t>Кубок Интретото</t>
+  </si>
+  <si>
+    <t>1996/97</t>
+  </si>
+  <si>
+    <t>Казбек</t>
+  </si>
+  <si>
+    <t>Махачкала</t>
+  </si>
+  <si>
+    <t>Олег Терёхин</t>
+  </si>
+  <si>
+    <t>Олег Кононов</t>
+  </si>
+  <si>
+    <t>Марко ван Бастен</t>
+  </si>
+  <si>
+    <t>Рашид Рахимов</t>
+  </si>
+  <si>
+    <t>Грозная Арена</t>
+  </si>
+  <si>
+    <t>Дракон</t>
+  </si>
+  <si>
+    <t>Умар Садаев</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Виталий Якушкин </t>
+  </si>
+  <si>
+    <t>Минкаил Мацуев</t>
+  </si>
+  <si>
+    <t>Лечи Садулаев</t>
+  </si>
+  <si>
+    <t>Амин Талаль</t>
+  </si>
+  <si>
+    <t>Михаил Ахмедов</t>
+  </si>
+  <si>
+    <t>Владислав Камилов</t>
+  </si>
+  <si>
+    <t>num_4</t>
+  </si>
+  <si>
+    <t>4-е</t>
+  </si>
+  <si>
+    <t>Лига Европы</t>
+  </si>
+  <si>
+    <t>2009/10</t>
+  </si>
+  <si>
+    <t>Ставрополь</t>
+  </si>
+  <si>
+    <t>Виктор Булатов</t>
+  </si>
+  <si>
+    <t>Станислав Черчесов</t>
+  </si>
+  <si>
+    <t>Лотар Маттеус</t>
+  </si>
+  <si>
+    <t>Магомед Даудов</t>
+  </si>
+  <si>
+    <t>Кадыров Стэдиум</t>
+  </si>
+  <si>
+    <t>Орёл</t>
+  </si>
+  <si>
+    <t>Магомед Якуев</t>
+  </si>
+  <si>
+    <t>Турпал-Али Ибишев</t>
+  </si>
+  <si>
+    <t>num_7</t>
+  </si>
+  <si>
+    <t>7-е</t>
+  </si>
+  <si>
+    <t>Лига Конференций</t>
+  </si>
+  <si>
+    <t>1994/95</t>
+  </si>
+  <si>
+    <t>Вайнах</t>
+  </si>
+  <si>
+    <t>Владикавказ</t>
+  </si>
+  <si>
+    <t>Андрей Каряка</t>
+  </si>
+  <si>
+    <t>Игорь Беланов</t>
+  </si>
+  <si>
+    <t>Ахмат Кадыров</t>
+  </si>
+  <si>
+    <t>Арена Терек</t>
+  </si>
+  <si>
+    <t>Сокол</t>
   </si>
   <si>
     <t>Магомед Адиев</t>
   </si>
   <si>
-    <t>Гамид Агаларов</t>
-  </si>
-  <si>
-    <t>Бернард Бериша</t>
-  </si>
-  <si>
-    <t>Гиорги Шелия</t>
-  </si>
-  <si>
-    <t>Антон Швец</t>
-  </si>
-  <si>
-    <t>Камило</t>
-  </si>
-  <si>
-    <t>Мирослав Богосовац</t>
-  </si>
-  <si>
-    <t>Надер Гандри</t>
-  </si>
-  <si>
-    <t>Лукас Ловат</t>
-  </si>
-  <si>
-    <t>Дарко Тодорович</t>
-  </si>
-  <si>
-    <t>Амин Талал</t>
-  </si>
-  <si>
-    <t>Заим Диванович</t>
-  </si>
-  <si>
-    <t>Милош Шатара</t>
-  </si>
-  <si>
-    <t>Евгений Харин</t>
-  </si>
-  <si>
-    <t>Исмаэл Силва</t>
-  </si>
-  <si>
-    <t>Феллипе Кардозо</t>
-  </si>
-  <si>
-    <t>Мауро Луна</t>
-  </si>
-  <si>
-    <t>Светослав Ковачев</t>
-  </si>
-  <si>
-    <t>num_6</t>
-  </si>
-  <si>
-    <t>6-е</t>
-  </si>
-  <si>
-    <t>Кубок Интретото</t>
-  </si>
-  <si>
-    <t>1996/97</t>
-  </si>
-  <si>
-    <t>Казбек</t>
-  </si>
-  <si>
-    <t>Махачкала</t>
-  </si>
-  <si>
-    <t>Олег Терёхин</t>
-  </si>
-  <si>
-    <t>Олег Кононов</t>
-  </si>
-  <si>
-    <t>Марко ван Бастен</t>
-  </si>
-  <si>
-    <t>Рашид Рахимов</t>
-  </si>
-  <si>
-    <t>Грозная Арена</t>
-  </si>
-  <si>
-    <t>Дракон</t>
-  </si>
-  <si>
-    <t>Умар Садаев</t>
-  </si>
-  <si>
-    <t>Виталий Якушкин </t>
-  </si>
-  <si>
-    <t>Минкаил Мацуев</t>
-  </si>
-  <si>
-    <t>Лечи Садулаев</t>
-  </si>
-  <si>
-    <t>Амин Талаль</t>
-  </si>
-  <si>
-    <t>Михаил Ахмедов</t>
-  </si>
-  <si>
-    <t>Владислав Камилов</t>
-  </si>
-  <si>
-    <t>num_4</t>
-  </si>
-  <si>
-    <t>4-е</t>
-  </si>
-  <si>
-    <t>Лига Европы</t>
-  </si>
-  <si>
-    <t>2009/10</t>
-  </si>
-  <si>
-    <t>Ставрополь</t>
-  </si>
-  <si>
-    <t>Виктор Булатов</t>
-  </si>
-  <si>
-    <t>Станислав Черчесов</t>
-  </si>
-  <si>
-    <t>Лотар Маттеус</t>
-  </si>
-  <si>
-    <t>Магомед Даудов</t>
-  </si>
-  <si>
-    <t>Кадыров Стэдиум</t>
-  </si>
-  <si>
-    <t>Орёл</t>
-  </si>
-  <si>
-    <t>Магомед Якуев</t>
-  </si>
-  <si>
-    <t>Турпал-Али Ибишев</t>
-  </si>
-  <si>
-    <t>num_7</t>
-  </si>
-  <si>
-    <t>7-е</t>
-  </si>
-  <si>
-    <t>Лига Конференций</t>
-  </si>
-  <si>
-    <t>1994/95</t>
-  </si>
-  <si>
-    <t>Вайнах</t>
-  </si>
-  <si>
-    <t>Владикавказ</t>
-  </si>
-  <si>
-    <t>Андрей Каряка</t>
-  </si>
-  <si>
-    <t>Игорь Беланов</t>
-  </si>
-  <si>
-    <t>Ахмат Кадыров</t>
-  </si>
-  <si>
-    <t>Арена Терек</t>
-  </si>
-  <si>
-    <t>Сокол</t>
-  </si>
-  <si>
     <t>Яхья Магомедов</t>
   </si>
   <si>
@@ -507,7 +511,7 @@
     <t>Христо Стоичков</t>
   </si>
   <si>
-    <t> Магомед Адиев</t>
+    <t xml:space="preserve"> Магомед Адиев</t>
   </si>
   <si>
     <t>Каспийская</t>
@@ -556,22 +560,13 @@
   </si>
   <si>
     <t>Абубакар Иналкаев</t>
-  </si>
-  <si>
-    <t>akh_samorodov</t>
-  </si>
-  <si>
-    <t>22-летний(29.06.2002) казахский нападающий. Перешёл в Ахмат летом 2024 из Актобе</t>
-  </si>
-  <si>
-    <t>Максим Самородов</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -630,25 +625,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -686,9 +673,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -720,10 +707,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,10 +741,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -931,21 +916,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="135.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -998,7 +976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1009,49 +987,49 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
         <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="L2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="M2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="N2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="O2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="P2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="Q2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1062,49 +1040,49 @@
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
         <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="J3" t="s">
         <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L3" t="s">
         <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N3" t="s">
         <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="P3" t="s">
         <v>34</v>
       </c>
       <c r="Q3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1115,7 +1093,7 @@
         <v>35</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E4" t="s">
         <v>35</v>
@@ -1124,40 +1102,40 @@
         <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="J4" t="s">
         <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L4" t="s">
         <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
       </c>
       <c r="O4" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1168,7 +1146,7 @@
         <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
         <v>35</v>
@@ -1177,40 +1155,40 @@
         <v>34</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H5" t="s">
         <v>34</v>
       </c>
       <c r="I5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="J5" t="s">
         <v>34</v>
       </c>
       <c r="K5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L5" t="s">
         <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="N5" t="s">
         <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="P5" t="s">
         <v>34</v>
       </c>
       <c r="Q5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1227,40 +1205,40 @@
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="L6" t="s">
         <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="N6" t="s">
         <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="P6" t="s">
         <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1271,7 +1249,7 @@
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
         <v>35</v>
@@ -1280,40 +1258,40 @@
         <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="L7" t="s">
         <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="N7" t="s">
         <v>34</v>
       </c>
       <c r="O7" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="P7" t="s">
         <v>34</v>
       </c>
       <c r="Q7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1354,16 +1332,16 @@
         <v>34</v>
       </c>
       <c r="O8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="P8" t="s">
         <v>34</v>
       </c>
       <c r="Q8" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1380,40 +1358,40 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H9" t="s">
         <v>34</v>
       </c>
       <c r="I9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J9" t="s">
         <v>34</v>
       </c>
       <c r="K9" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L9" t="s">
         <v>34</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="N9" t="s">
         <v>34</v>
       </c>
       <c r="O9" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="P9" t="s">
         <v>34</v>
       </c>
       <c r="Q9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1424,7 +1402,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E10" t="s">
         <v>35</v>
@@ -1433,40 +1411,40 @@
         <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J10" t="s">
         <v>34</v>
       </c>
       <c r="K10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L10" t="s">
         <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="N10" t="s">
         <v>34</v>
       </c>
       <c r="O10" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="P10" t="s">
         <v>34</v>
       </c>
       <c r="Q10" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1483,40 +1461,40 @@
         <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H11" t="s">
         <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J11" t="s">
         <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L11" t="s">
         <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="N11" t="s">
         <v>34</v>
       </c>
       <c r="O11" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="P11" t="s">
         <v>34</v>
       </c>
       <c r="Q11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1527,7 +1505,7 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
         <v>36</v>
@@ -1536,40 +1514,40 @@
         <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
         <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J12" t="s">
         <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L12" t="s">
         <v>34</v>
       </c>
       <c r="M12" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="N12" t="s">
         <v>34</v>
       </c>
       <c r="O12" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="P12" t="s">
         <v>34</v>
       </c>
       <c r="Q12" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1580,46 +1558,46 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
       </c>
       <c r="I13" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J13" t="s">
         <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L13" t="s">
         <v>34</v>
       </c>
       <c r="M13" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="N13" t="s">
         <v>34</v>
       </c>
       <c r="O13" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="P13" t="s">
         <v>34</v>
       </c>
       <c r="Q13" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1630,7 +1608,7 @@
         <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
         <v>49</v>
@@ -1639,40 +1617,40 @@
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H14" t="s">
         <v>45</v>
       </c>
       <c r="I14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J14" t="s">
         <v>40</v>
       </c>
       <c r="K14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L14" t="s">
         <v>38</v>
       </c>
       <c r="M14" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="N14" t="s">
         <v>39</v>
       </c>
       <c r="O14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P14" t="s">
         <v>37</v>
       </c>
       <c r="Q14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1683,7 +1661,7 @@
         <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
@@ -1692,40 +1670,40 @@
         <v>34</v>
       </c>
       <c r="G15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
       </c>
       <c r="I15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J15" t="s">
         <v>34</v>
       </c>
       <c r="K15" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L15" t="s">
         <v>34</v>
       </c>
       <c r="M15" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
       <c r="N15" t="s">
         <v>34</v>
       </c>
       <c r="O15" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="P15" t="s">
         <v>34</v>
       </c>
       <c r="Q15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1736,7 +1714,7 @@
         <v>35</v>
       </c>
       <c r="D16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" t="s">
         <v>35</v>
@@ -1745,40 +1723,40 @@
         <v>34</v>
       </c>
       <c r="G16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" t="s">
+        <v>122</v>
+      </c>
+      <c r="J16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" t="s">
+        <v>92</v>
+      </c>
+      <c r="L16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" t="s">
         <v>88</v>
       </c>
-      <c r="H16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I16" t="s">
-        <v>120</v>
-      </c>
-      <c r="J16" t="s">
-        <v>34</v>
-      </c>
-      <c r="K16" t="s">
-        <v>91</v>
-      </c>
-      <c r="L16" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" t="s">
-        <v>86</v>
-      </c>
       <c r="N16" t="s">
         <v>34</v>
       </c>
       <c r="O16" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="P16" t="s">
         <v>34</v>
       </c>
       <c r="Q16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1789,7 +1767,7 @@
         <v>35</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
         <v>35</v>
@@ -1831,7 +1809,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1842,7 +1820,7 @@
         <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
         <v>37</v>
@@ -1851,40 +1829,40 @@
         <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H18" t="s">
         <v>34</v>
       </c>
       <c r="I18" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L18" t="s">
         <v>34</v>
       </c>
       <c r="M18" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="N18" t="s">
         <v>34</v>
       </c>
       <c r="O18" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="P18" t="s">
         <v>34</v>
       </c>
       <c r="Q18" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1895,7 +1873,7 @@
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E19" t="s">
         <v>38</v>
@@ -1904,40 +1882,40 @@
         <v>34</v>
       </c>
       <c r="G19" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H19" t="s">
         <v>34</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J19" t="s">
         <v>34</v>
       </c>
       <c r="K19" t="s">
+        <v>102</v>
+      </c>
+      <c r="L19" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" t="s">
+        <v>153</v>
+      </c>
+      <c r="N19" t="s">
+        <v>34</v>
+      </c>
+      <c r="O19" t="s">
         <v>101</v>
       </c>
-      <c r="L19" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" t="s">
-        <v>150</v>
-      </c>
-      <c r="N19" t="s">
-        <v>34</v>
-      </c>
-      <c r="O19" t="s">
-        <v>100</v>
-      </c>
       <c r="P19" t="s">
         <v>34</v>
       </c>
       <c r="Q19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1948,7 +1926,7 @@
         <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
         <v>39</v>
@@ -1957,40 +1935,40 @@
         <v>34</v>
       </c>
       <c r="G20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H20" t="s">
         <v>34</v>
       </c>
       <c r="I20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J20" t="s">
         <v>34</v>
       </c>
       <c r="K20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L20" t="s">
         <v>34</v>
       </c>
       <c r="M20" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N20" t="s">
         <v>34</v>
       </c>
       <c r="O20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="P20" t="s">
         <v>34</v>
       </c>
       <c r="Q20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2001,7 +1979,7 @@
         <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
         <v>40</v>
@@ -2010,40 +1988,40 @@
         <v>34</v>
       </c>
       <c r="G21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H21" t="s">
         <v>34</v>
       </c>
       <c r="I21" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J21" t="s">
         <v>34</v>
       </c>
       <c r="K21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L21" t="s">
         <v>34</v>
       </c>
       <c r="M21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N21" t="s">
         <v>34</v>
       </c>
       <c r="O21" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="P21" t="s">
         <v>34</v>
       </c>
       <c r="Q21" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2054,7 +2032,7 @@
         <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E22" t="s">
         <v>41</v>
@@ -2063,40 +2041,40 @@
         <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H22" t="s">
         <v>34</v>
       </c>
       <c r="I22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J22" t="s">
         <v>34</v>
       </c>
       <c r="K22" t="s">
+        <v>98</v>
+      </c>
+      <c r="L22" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" t="s">
         <v>97</v>
       </c>
-      <c r="L22" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" t="s">
-        <v>96</v>
-      </c>
       <c r="N22" t="s">
         <v>34</v>
       </c>
       <c r="O22" t="s">
+        <v>102</v>
+      </c>
+      <c r="P22" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" t="s">
         <v>101</v>
       </c>
-      <c r="P22" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2107,7 +2085,7 @@
         <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E23" t="s">
         <v>42</v>
@@ -2116,40 +2094,40 @@
         <v>34</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H23" t="s">
         <v>34</v>
       </c>
       <c r="I23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J23" t="s">
         <v>34</v>
       </c>
       <c r="K23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L23" t="s">
         <v>34</v>
       </c>
       <c r="M23" t="s">
+        <v>92</v>
+      </c>
+      <c r="N23" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" t="s">
         <v>91</v>
       </c>
-      <c r="N23" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" t="s">
-        <v>90</v>
-      </c>
       <c r="P23" t="s">
         <v>34</v>
       </c>
       <c r="Q23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2160,7 +2138,7 @@
         <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E24" t="s">
         <v>43</v>
@@ -2169,40 +2147,40 @@
         <v>34</v>
       </c>
       <c r="G24" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H24" t="s">
         <v>34</v>
       </c>
       <c r="I24" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J24" t="s">
         <v>34</v>
       </c>
       <c r="K24" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L24" t="s">
         <v>34</v>
       </c>
       <c r="M24" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="N24" t="s">
         <v>34</v>
       </c>
       <c r="O24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P24" t="s">
         <v>34</v>
       </c>
       <c r="Q24" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2213,7 +2191,7 @@
         <v>44</v>
       </c>
       <c r="D25" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E25" t="s">
         <v>44</v>
@@ -2222,40 +2200,40 @@
         <v>34</v>
       </c>
       <c r="G25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" t="s">
+        <v>34</v>
+      </c>
+      <c r="I25" t="s">
+        <v>99</v>
+      </c>
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+      <c r="K25" t="s">
         <v>97</v>
       </c>
-      <c r="H25" t="s">
-        <v>34</v>
-      </c>
-      <c r="I25" t="s">
-        <v>98</v>
-      </c>
-      <c r="J25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K25" t="s">
+      <c r="L25" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" t="s">
         <v>96</v>
       </c>
-      <c r="L25" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
+        <v>34</v>
+      </c>
+      <c r="O25" t="s">
         <v>95</v>
       </c>
-      <c r="N25" t="s">
-        <v>34</v>
-      </c>
-      <c r="O25" t="s">
-        <v>94</v>
-      </c>
       <c r="P25" t="s">
         <v>34</v>
       </c>
       <c r="Q25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2266,7 +2244,7 @@
         <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
         <v>45</v>
@@ -2275,40 +2253,40 @@
         <v>34</v>
       </c>
       <c r="G26" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H26" t="s">
         <v>34</v>
       </c>
       <c r="I26" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J26" t="s">
         <v>34</v>
       </c>
       <c r="K26" t="s">
+        <v>96</v>
+      </c>
+      <c r="L26" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" t="s">
+        <v>94</v>
+      </c>
+      <c r="N26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" t="s">
+        <v>91</v>
+      </c>
+      <c r="P26" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q26" t="s">
         <v>95</v>
       </c>
-      <c r="L26" t="s">
-        <v>34</v>
-      </c>
-      <c r="M26" t="s">
-        <v>93</v>
-      </c>
-      <c r="N26" t="s">
-        <v>34</v>
-      </c>
-      <c r="O26" t="s">
-        <v>90</v>
-      </c>
-      <c r="P26" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2319,7 +2297,7 @@
         <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
         <v>46</v>
@@ -2328,40 +2306,40 @@
         <v>34</v>
       </c>
       <c r="G27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H27" t="s">
         <v>34</v>
       </c>
       <c r="I27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J27" t="s">
         <v>34</v>
       </c>
       <c r="K27" t="s">
+        <v>98</v>
+      </c>
+      <c r="L27" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" t="s">
         <v>97</v>
       </c>
-      <c r="L27" t="s">
-        <v>34</v>
-      </c>
-      <c r="M27" t="s">
-        <v>96</v>
-      </c>
       <c r="N27" t="s">
         <v>34</v>
       </c>
       <c r="O27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P27" t="s">
         <v>34</v>
       </c>
       <c r="Q27" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2372,7 +2350,7 @@
         <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
@@ -2381,40 +2359,40 @@
         <v>34</v>
       </c>
       <c r="G28" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H28" t="s">
         <v>34</v>
       </c>
       <c r="I28" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J28" t="s">
         <v>34</v>
       </c>
       <c r="K28" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L28" t="s">
         <v>34</v>
       </c>
       <c r="M28" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="N28" t="s">
         <v>34</v>
       </c>
       <c r="O28" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="P28" t="s">
         <v>34</v>
       </c>
       <c r="Q28" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2425,7 +2403,7 @@
         <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
         <v>48</v>
@@ -2434,40 +2412,40 @@
         <v>34</v>
       </c>
       <c r="G29" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
       </c>
       <c r="I29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29" t="s">
+        <v>34</v>
+      </c>
+      <c r="M29" t="s">
         <v>98</v>
       </c>
-      <c r="J29" t="s">
-        <v>34</v>
-      </c>
-      <c r="K29" t="s">
-        <v>95</v>
-      </c>
-      <c r="L29" t="s">
-        <v>34</v>
-      </c>
-      <c r="M29" t="s">
-        <v>97</v>
-      </c>
       <c r="N29" t="s">
         <v>34</v>
       </c>
       <c r="O29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="P29" t="s">
         <v>34</v>
       </c>
       <c r="Q29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2478,7 +2456,7 @@
         <v>49</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
         <v>49</v>
@@ -2487,40 +2465,40 @@
         <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H30" t="s">
         <v>34</v>
       </c>
       <c r="I30" t="s">
+        <v>126</v>
+      </c>
+      <c r="J30" t="s">
+        <v>34</v>
+      </c>
+      <c r="K30" t="s">
+        <v>140</v>
+      </c>
+      <c r="L30" t="s">
+        <v>34</v>
+      </c>
+      <c r="M30" t="s">
+        <v>139</v>
+      </c>
+      <c r="N30" t="s">
+        <v>34</v>
+      </c>
+      <c r="O30" t="s">
         <v>124</v>
       </c>
-      <c r="J30" t="s">
-        <v>34</v>
-      </c>
-      <c r="K30" t="s">
-        <v>138</v>
-      </c>
-      <c r="L30" t="s">
-        <v>34</v>
-      </c>
-      <c r="M30" t="s">
-        <v>137</v>
-      </c>
-      <c r="N30" t="s">
-        <v>34</v>
-      </c>
-      <c r="O30" t="s">
-        <v>122</v>
-      </c>
       <c r="P30" t="s">
         <v>34</v>
       </c>
       <c r="Q30" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2531,7 +2509,7 @@
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E31" t="s">
         <v>50</v>
@@ -2540,40 +2518,40 @@
         <v>34</v>
       </c>
       <c r="G31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H31" t="s">
         <v>34</v>
       </c>
       <c r="I31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="J31" t="s">
         <v>34</v>
       </c>
       <c r="K31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L31" t="s">
         <v>34</v>
       </c>
       <c r="M31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N31" t="s">
         <v>34</v>
       </c>
       <c r="O31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="P31" t="s">
         <v>34</v>
       </c>
       <c r="Q31" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2584,7 +2562,7 @@
         <v>51</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
         <v>51</v>
@@ -2593,40 +2571,40 @@
         <v>34</v>
       </c>
       <c r="G32" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H32" t="s">
         <v>34</v>
       </c>
       <c r="I32" t="s">
+        <v>98</v>
+      </c>
+      <c r="J32" t="s">
+        <v>34</v>
+      </c>
+      <c r="K32" t="s">
+        <v>102</v>
+      </c>
+      <c r="L32" t="s">
+        <v>34</v>
+      </c>
+      <c r="M32" t="s">
+        <v>95</v>
+      </c>
+      <c r="N32" t="s">
+        <v>34</v>
+      </c>
+      <c r="O32" t="s">
         <v>97</v>
       </c>
-      <c r="J32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K32" t="s">
-        <v>101</v>
-      </c>
-      <c r="L32" t="s">
-        <v>34</v>
-      </c>
-      <c r="M32" t="s">
-        <v>94</v>
-      </c>
-      <c r="N32" t="s">
-        <v>34</v>
-      </c>
-      <c r="O32" t="s">
-        <v>96</v>
-      </c>
       <c r="P32" t="s">
         <v>34</v>
       </c>
       <c r="Q32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2637,7 +2615,7 @@
         <v>52</v>
       </c>
       <c r="D33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E33" t="s">
         <v>52</v>
@@ -2646,40 +2624,40 @@
         <v>34</v>
       </c>
       <c r="G33" t="s">
+        <v>105</v>
+      </c>
+      <c r="H33" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" t="s">
         <v>104</v>
       </c>
-      <c r="H33" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" t="s">
-        <v>103</v>
-      </c>
       <c r="J33" t="s">
         <v>34</v>
       </c>
       <c r="K33" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L33" t="s">
         <v>34</v>
       </c>
       <c r="M33" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N33" t="s">
         <v>34</v>
       </c>
       <c r="O33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="P33" t="s">
         <v>34</v>
       </c>
       <c r="Q33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2690,7 +2668,7 @@
         <v>53</v>
       </c>
       <c r="D34" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E34" t="s">
         <v>53</v>
@@ -2699,40 +2677,40 @@
         <v>34</v>
       </c>
       <c r="G34" t="s">
+        <v>106</v>
+      </c>
+      <c r="H34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" t="s">
         <v>105</v>
       </c>
-      <c r="H34" t="s">
-        <v>34</v>
-      </c>
-      <c r="I34" t="s">
-        <v>103</v>
-      </c>
-      <c r="J34" t="s">
-        <v>34</v>
-      </c>
-      <c r="K34" t="s">
-        <v>104</v>
-      </c>
       <c r="L34" t="s">
         <v>34</v>
       </c>
       <c r="M34" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N34" t="s">
         <v>34</v>
       </c>
       <c r="O34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="P34" t="s">
         <v>34</v>
       </c>
       <c r="Q34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2743,7 +2721,7 @@
         <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
         <v>54</v>
@@ -2752,40 +2730,40 @@
         <v>34</v>
       </c>
       <c r="G35" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H35" t="s">
         <v>34</v>
       </c>
       <c r="I35" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J35" t="s">
         <v>34</v>
       </c>
       <c r="K35" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L35" t="s">
         <v>34</v>
       </c>
       <c r="M35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N35" t="s">
         <v>34</v>
       </c>
       <c r="O35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="P35" t="s">
         <v>34</v>
       </c>
       <c r="Q35" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>1</v>
       </c>
@@ -2793,49 +2771,49 @@
         <v>33</v>
       </c>
       <c r="C36" t="s">
-        <v>179</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>179</v>
+        <v>55</v>
       </c>
       <c r="F36" t="s">
         <v>34</v>
       </c>
       <c r="G36" t="s">
-        <v>181</v>
+        <v>108</v>
       </c>
       <c r="H36" t="s">
         <v>34</v>
       </c>
       <c r="I36" t="s">
+        <v>103</v>
+      </c>
+      <c r="J36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K36" t="s">
+        <v>107</v>
+      </c>
+      <c r="L36" t="s">
+        <v>34</v>
+      </c>
+      <c r="M36" t="s">
         <v>102</v>
       </c>
-      <c r="J36" t="s">
-        <v>34</v>
-      </c>
-      <c r="K36" t="s">
-        <v>106</v>
-      </c>
-      <c r="L36" t="s">
-        <v>34</v>
-      </c>
-      <c r="M36" t="s">
-        <v>101</v>
-      </c>
       <c r="N36" t="s">
         <v>34</v>
       </c>
       <c r="O36" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="P36" t="s">
         <v>34</v>
       </c>
       <c r="Q36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add 05 09 @SvyTo
</commit_message>
<xml_diff>
--- a/RPL_V2/xlsx/club_akhmat.xlsx
+++ b/RPL_V2/xlsx/club_akhmat.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SvyTo\PycharmProjects\amaranth64.github.io\RPL_V2\xlsx\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="181">
   <si>
     <t>type</t>
   </si>
@@ -217,9 +222,6 @@
     <t>Ведёт свою историю с 1946 года</t>
   </si>
   <si>
-    <t>Нападающий</t>
-  </si>
-  <si>
     <t>Полузащитник</t>
   </si>
   <si>
@@ -286,7 +288,7 @@
     <t>Виталий Якушкин</t>
   </si>
   <si>
-    <t xml:space="preserve"> Анатолий Синько</t>
+    <t> Анатолий Синько</t>
   </si>
   <si>
     <t>Гамид Агаларов</t>
@@ -382,7 +384,7 @@
     <t>Умар Садаев</t>
   </si>
   <si>
-    <t xml:space="preserve">Виталий Якушкин </t>
+    <t>Виталий Якушкин </t>
   </si>
   <si>
     <t>Минкаил Мацуев</t>
@@ -511,7 +513,7 @@
     <t>Христо Стоичков</t>
   </si>
   <si>
-    <t xml:space="preserve"> Магомед Адиев</t>
+    <t> Магомед Адиев</t>
   </si>
   <si>
     <t>Каспийская</t>
@@ -565,8 +567,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,17 +627,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -673,9 +683,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -707,9 +717,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -741,9 +752,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -916,14 +928,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,7 +993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4</v>
       </c>
@@ -993,43 +1010,43 @@
         <v>35</v>
       </c>
       <c r="F2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" t="s">
         <v>77</v>
       </c>
-      <c r="G2" t="s">
-        <v>78</v>
-      </c>
       <c r="H2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" t="s">
         <v>109</v>
       </c>
-      <c r="I2" t="s">
-        <v>110</v>
-      </c>
       <c r="J2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" t="s">
         <v>128</v>
       </c>
-      <c r="K2" t="s">
-        <v>129</v>
-      </c>
       <c r="L2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" t="s">
         <v>141</v>
       </c>
-      <c r="M2" t="s">
-        <v>142</v>
-      </c>
       <c r="N2" t="s">
+        <v>154</v>
+      </c>
+      <c r="O2" t="s">
         <v>155</v>
       </c>
-      <c r="O2" t="s">
-        <v>156</v>
-      </c>
       <c r="P2" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q2" t="s">
         <v>170</v>
       </c>
-      <c r="Q2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1043,7 +1060,7 @@
         <v>57</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" t="s">
         <v>34</v>
@@ -1055,34 +1072,34 @@
         <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J3" t="s">
         <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L3" t="s">
         <v>34</v>
       </c>
       <c r="M3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N3" t="s">
         <v>34</v>
       </c>
       <c r="O3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="P3" t="s">
         <v>34</v>
       </c>
       <c r="Q3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1102,40 +1119,40 @@
         <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J4" t="s">
         <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="L4" t="s">
         <v>34</v>
       </c>
       <c r="M4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
       </c>
       <c r="O4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P4" t="s">
         <v>34</v>
       </c>
       <c r="Q4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1155,40 +1172,40 @@
         <v>34</v>
       </c>
       <c r="G5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
         <v>80</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>113</v>
-      </c>
-      <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>81</v>
-      </c>
       <c r="L5" t="s">
         <v>34</v>
       </c>
       <c r="M5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N5" t="s">
         <v>34</v>
       </c>
       <c r="O5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="P5" t="s">
         <v>34</v>
       </c>
       <c r="Q5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1205,40 +1222,40 @@
         <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
         <v>34</v>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J6" t="s">
         <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L6" t="s">
         <v>34</v>
       </c>
       <c r="M6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N6" t="s">
         <v>34</v>
       </c>
       <c r="O6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="P6" t="s">
         <v>34</v>
       </c>
       <c r="Q6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1258,40 +1275,40 @@
         <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="I7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J7" t="s">
         <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L7" t="s">
         <v>34</v>
       </c>
       <c r="M7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N7" t="s">
         <v>34</v>
       </c>
       <c r="O7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="P7" t="s">
         <v>34</v>
       </c>
       <c r="Q7" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1332,16 +1349,16 @@
         <v>34</v>
       </c>
       <c r="O8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P8" t="s">
         <v>34</v>
       </c>
       <c r="Q8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1358,40 +1375,40 @@
         <v>34</v>
       </c>
       <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>115</v>
+      </c>
+      <c r="J9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" t="s">
         <v>83</v>
       </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" t="s">
-        <v>116</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
-      </c>
-      <c r="K9" t="s">
-        <v>134</v>
-      </c>
-      <c r="L9" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" t="s">
-        <v>84</v>
-      </c>
       <c r="N9" t="s">
         <v>34</v>
       </c>
       <c r="O9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P9" t="s">
         <v>34</v>
       </c>
       <c r="Q9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1411,40 +1428,40 @@
         <v>34</v>
       </c>
       <c r="G10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H10" t="s">
         <v>34</v>
       </c>
       <c r="I10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J10" t="s">
         <v>34</v>
       </c>
       <c r="K10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="L10" t="s">
         <v>34</v>
       </c>
       <c r="M10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N10" t="s">
         <v>34</v>
       </c>
       <c r="O10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P10" t="s">
         <v>34</v>
       </c>
       <c r="Q10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1461,40 +1478,40 @@
         <v>34</v>
       </c>
       <c r="G11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" t="s">
         <v>34</v>
       </c>
       <c r="I11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J11" t="s">
         <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L11" t="s">
         <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N11" t="s">
         <v>34</v>
       </c>
       <c r="O11" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P11" t="s">
         <v>34</v>
       </c>
       <c r="Q11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1514,40 +1531,40 @@
         <v>34</v>
       </c>
       <c r="G12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H12" t="s">
         <v>34</v>
       </c>
       <c r="I12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J12" t="s">
         <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L12" t="s">
         <v>34</v>
       </c>
       <c r="M12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N12" t="s">
         <v>34</v>
       </c>
       <c r="O12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P12" t="s">
         <v>34</v>
       </c>
       <c r="Q12" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1558,46 +1575,46 @@
         <v>35</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
       </c>
       <c r="G13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H13" t="s">
         <v>34</v>
       </c>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J13" t="s">
         <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L13" t="s">
         <v>34</v>
       </c>
       <c r="M13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="N13" t="s">
         <v>34</v>
       </c>
       <c r="O13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P13" t="s">
         <v>34</v>
       </c>
       <c r="Q13" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1617,40 +1634,40 @@
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" t="s">
         <v>45</v>
       </c>
       <c r="I14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J14" t="s">
         <v>40</v>
       </c>
       <c r="K14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L14" t="s">
         <v>38</v>
       </c>
       <c r="M14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="N14" t="s">
         <v>39</v>
       </c>
       <c r="O14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P14" t="s">
         <v>37</v>
       </c>
       <c r="Q14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1670,40 +1687,40 @@
         <v>34</v>
       </c>
       <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>34</v>
+      </c>
+      <c r="I15" t="s">
+        <v>120</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" t="s">
+        <v>81</v>
+      </c>
+      <c r="L15" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" t="s">
+        <v>151</v>
+      </c>
+      <c r="N15" t="s">
+        <v>34</v>
+      </c>
+      <c r="O15" t="s">
+        <v>132</v>
+      </c>
+      <c r="P15" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15" t="s">
         <v>89</v>
       </c>
-      <c r="H15" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" t="s">
-        <v>121</v>
-      </c>
-      <c r="J15" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" t="s">
-        <v>82</v>
-      </c>
-      <c r="L15" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" t="s">
-        <v>152</v>
-      </c>
-      <c r="N15" t="s">
-        <v>34</v>
-      </c>
-      <c r="O15" t="s">
-        <v>133</v>
-      </c>
-      <c r="P15" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1723,40 +1740,40 @@
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
       </c>
       <c r="I16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J16" t="s">
         <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L16" t="s">
         <v>34</v>
       </c>
       <c r="M16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N16" t="s">
         <v>34</v>
       </c>
       <c r="O16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="P16" t="s">
         <v>34</v>
       </c>
       <c r="Q16" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1809,7 +1826,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1817,13 +1834,13 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
         <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F18" t="s">
         <v>34</v>
@@ -1835,34 +1852,34 @@
         <v>34</v>
       </c>
       <c r="I18" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="J18" t="s">
         <v>34</v>
       </c>
       <c r="K18" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="L18" t="s">
         <v>34</v>
       </c>
       <c r="M18" t="s">
-        <v>124</v>
+        <v>152</v>
       </c>
       <c r="N18" t="s">
         <v>34</v>
       </c>
       <c r="O18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="P18" t="s">
         <v>34</v>
       </c>
       <c r="Q18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1870,13 +1887,13 @@
         <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
         <v>68</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F19" t="s">
         <v>34</v>
@@ -1888,13 +1905,13 @@
         <v>34</v>
       </c>
       <c r="I19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J19" t="s">
         <v>34</v>
       </c>
       <c r="K19" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="L19" t="s">
         <v>34</v>
@@ -1906,16 +1923,16 @@
         <v>34</v>
       </c>
       <c r="O19" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
       <c r="P19" t="s">
         <v>34</v>
       </c>
       <c r="Q19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1923,13 +1940,13 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F20" t="s">
         <v>34</v>
@@ -1941,34 +1958,34 @@
         <v>34</v>
       </c>
       <c r="I20" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="J20" t="s">
         <v>34</v>
       </c>
       <c r="K20" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="L20" t="s">
         <v>34</v>
       </c>
       <c r="M20" t="s">
-        <v>154</v>
+        <v>106</v>
       </c>
       <c r="N20" t="s">
         <v>34</v>
       </c>
       <c r="O20" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
       <c r="P20" t="s">
         <v>34</v>
       </c>
       <c r="Q20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1976,13 +1993,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
         <v>34</v>
@@ -2000,28 +2017,28 @@
         <v>34</v>
       </c>
       <c r="K21" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="L21" t="s">
         <v>34</v>
       </c>
       <c r="M21" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="N21" t="s">
         <v>34</v>
       </c>
       <c r="O21" t="s">
-        <v>168</v>
+        <v>101</v>
       </c>
       <c r="P21" t="s">
         <v>34</v>
       </c>
       <c r="Q21" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2029,13 +2046,13 @@
         <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F22" t="s">
         <v>34</v>
@@ -2047,7 +2064,7 @@
         <v>34</v>
       </c>
       <c r="I22" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="J22" t="s">
         <v>34</v>
@@ -2059,22 +2076,22 @@
         <v>34</v>
       </c>
       <c r="M22" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="N22" t="s">
         <v>34</v>
       </c>
       <c r="O22" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="P22" t="s">
         <v>34</v>
       </c>
       <c r="Q22" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2082,13 +2099,13 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D23" t="s">
         <v>63</v>
       </c>
       <c r="E23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
         <v>34</v>
@@ -2100,34 +2117,34 @@
         <v>34</v>
       </c>
       <c r="I23" t="s">
+        <v>97</v>
+      </c>
+      <c r="J23" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" t="s">
+        <v>98</v>
+      </c>
+      <c r="L23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" t="s">
+        <v>124</v>
+      </c>
+      <c r="N23" t="s">
+        <v>34</v>
+      </c>
+      <c r="O23" t="s">
         <v>101</v>
       </c>
-      <c r="J23" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" t="s">
-        <v>99</v>
-      </c>
-      <c r="L23" t="s">
-        <v>34</v>
-      </c>
-      <c r="M23" t="s">
-        <v>92</v>
-      </c>
-      <c r="N23" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" t="s">
+      <c r="P23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q23" t="s">
         <v>91</v>
       </c>
-      <c r="P23" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17">
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2135,13 +2152,13 @@
         <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s">
         <v>63</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F24" t="s">
         <v>34</v>
@@ -2159,28 +2176,28 @@
         <v>34</v>
       </c>
       <c r="K24" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L24" t="s">
         <v>34</v>
       </c>
       <c r="M24" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="N24" t="s">
         <v>34</v>
       </c>
       <c r="O24" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="P24" t="s">
         <v>34</v>
       </c>
       <c r="Q24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -2188,13 +2205,13 @@
         <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D25" t="s">
         <v>63</v>
       </c>
       <c r="E25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s">
         <v>34</v>
@@ -2206,34 +2223,34 @@
         <v>34</v>
       </c>
       <c r="I25" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J25" t="s">
         <v>34</v>
       </c>
       <c r="K25" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L25" t="s">
         <v>34</v>
       </c>
       <c r="M25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N25" t="s">
         <v>34</v>
       </c>
       <c r="O25" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="P25" t="s">
         <v>34</v>
       </c>
       <c r="Q25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2241,13 +2258,13 @@
         <v>33</v>
       </c>
       <c r="C26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
         <v>34</v>
@@ -2259,34 +2276,34 @@
         <v>34</v>
       </c>
       <c r="I26" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J26" t="s">
         <v>34</v>
       </c>
       <c r="K26" t="s">
+        <v>97</v>
+      </c>
+      <c r="L26" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" t="s">
         <v>96</v>
       </c>
-      <c r="L26" t="s">
-        <v>34</v>
-      </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
+        <v>34</v>
+      </c>
+      <c r="O26" t="s">
         <v>94</v>
       </c>
-      <c r="N26" t="s">
-        <v>34</v>
-      </c>
-      <c r="O26" t="s">
-        <v>91</v>
-      </c>
       <c r="P26" t="s">
         <v>34</v>
       </c>
       <c r="Q26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -2294,13 +2311,13 @@
         <v>33</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s">
         <v>34</v>
@@ -2312,25 +2329,25 @@
         <v>34</v>
       </c>
       <c r="I27" t="s">
+        <v>92</v>
+      </c>
+      <c r="J27" t="s">
+        <v>34</v>
+      </c>
+      <c r="K27" t="s">
         <v>101</v>
       </c>
-      <c r="J27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K27" t="s">
-        <v>98</v>
-      </c>
       <c r="L27" t="s">
         <v>34</v>
       </c>
       <c r="M27" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="N27" t="s">
         <v>34</v>
       </c>
       <c r="O27" t="s">
-        <v>95</v>
+        <v>168</v>
       </c>
       <c r="P27" t="s">
         <v>34</v>
@@ -2339,7 +2356,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2347,13 +2364,13 @@
         <v>33</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F28" t="s">
         <v>34</v>
@@ -2365,34 +2382,34 @@
         <v>34</v>
       </c>
       <c r="I28" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J28" t="s">
         <v>34</v>
       </c>
       <c r="K28" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="L28" t="s">
         <v>34</v>
       </c>
       <c r="M28" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="N28" t="s">
         <v>34</v>
       </c>
       <c r="O28" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="P28" t="s">
         <v>34</v>
       </c>
       <c r="Q28" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2400,52 +2417,52 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
         <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F29" t="s">
         <v>34</v>
       </c>
       <c r="G29" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="H29" t="s">
         <v>34</v>
       </c>
       <c r="I29" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="J29" t="s">
         <v>34</v>
       </c>
       <c r="K29" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="L29" t="s">
         <v>34</v>
       </c>
       <c r="M29" t="s">
-        <v>98</v>
+        <v>138</v>
       </c>
       <c r="N29" t="s">
         <v>34</v>
       </c>
       <c r="O29" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="P29" t="s">
         <v>34</v>
       </c>
       <c r="Q29" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
@@ -2453,19 +2470,19 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
         <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H30" t="s">
         <v>34</v>
@@ -2477,28 +2494,28 @@
         <v>34</v>
       </c>
       <c r="K30" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="L30" t="s">
         <v>34</v>
       </c>
       <c r="M30" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="N30" t="s">
         <v>34</v>
       </c>
       <c r="O30" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="P30" t="s">
         <v>34</v>
       </c>
       <c r="Q30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2506,13 +2523,13 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="E31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F31" t="s">
         <v>34</v>
@@ -2524,34 +2541,34 @@
         <v>34</v>
       </c>
       <c r="I31" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
       <c r="J31" t="s">
         <v>34</v>
       </c>
       <c r="K31" t="s">
+        <v>101</v>
+      </c>
+      <c r="L31" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" t="s">
         <v>94</v>
       </c>
-      <c r="L31" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" t="s">
-        <v>91</v>
-      </c>
       <c r="N31" t="s">
         <v>34</v>
       </c>
       <c r="O31" t="s">
-        <v>139</v>
+        <v>96</v>
       </c>
       <c r="P31" t="s">
         <v>34</v>
       </c>
       <c r="Q31" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2559,13 +2576,13 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D32" t="s">
         <v>70</v>
       </c>
       <c r="E32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F32" t="s">
         <v>34</v>
@@ -2577,34 +2594,34 @@
         <v>34</v>
       </c>
       <c r="I32" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="J32" t="s">
         <v>34</v>
       </c>
       <c r="K32" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="L32" t="s">
         <v>34</v>
       </c>
       <c r="M32" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="N32" t="s">
         <v>34</v>
       </c>
       <c r="O32" t="s">
+        <v>94</v>
+      </c>
+      <c r="P32" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32" t="s">
         <v>97</v>
       </c>
-      <c r="P32" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17">
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2612,13 +2629,13 @@
         <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D33" t="s">
         <v>71</v>
       </c>
       <c r="E33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
         <v>34</v>
@@ -2630,25 +2647,25 @@
         <v>34</v>
       </c>
       <c r="I33" t="s">
+        <v>103</v>
+      </c>
+      <c r="J33" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" t="s">
         <v>104</v>
       </c>
-      <c r="J33" t="s">
-        <v>34</v>
-      </c>
-      <c r="K33" t="s">
+      <c r="L33" t="s">
+        <v>34</v>
+      </c>
+      <c r="M33" t="s">
         <v>106</v>
       </c>
-      <c r="L33" t="s">
-        <v>34</v>
-      </c>
-      <c r="M33" t="s">
-        <v>102</v>
-      </c>
       <c r="N33" t="s">
         <v>34</v>
       </c>
       <c r="O33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P33" t="s">
         <v>34</v>
@@ -2657,7 +2674,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2665,13 +2682,13 @@
         <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
         <v>72</v>
       </c>
       <c r="E34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F34" t="s">
         <v>34</v>
@@ -2683,34 +2700,34 @@
         <v>34</v>
       </c>
       <c r="I34" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J34" t="s">
         <v>34</v>
       </c>
       <c r="K34" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="L34" t="s">
         <v>34</v>
       </c>
       <c r="M34" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="N34" t="s">
         <v>34</v>
       </c>
       <c r="O34" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="P34" t="s">
         <v>34</v>
       </c>
       <c r="Q34" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
@@ -2718,13 +2735,13 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
         <v>73</v>
       </c>
       <c r="E35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F35" t="s">
         <v>34</v>
@@ -2736,84 +2753,31 @@
         <v>34</v>
       </c>
       <c r="I35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J35" t="s">
         <v>34</v>
       </c>
       <c r="K35" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="L35" t="s">
         <v>34</v>
       </c>
       <c r="M35" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="N35" t="s">
         <v>34</v>
       </c>
       <c r="O35" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="P35" t="s">
         <v>34</v>
       </c>
       <c r="Q35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C36" t="s">
-        <v>55</v>
-      </c>
-      <c r="D36" t="s">
-        <v>74</v>
-      </c>
-      <c r="E36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" t="s">
-        <v>34</v>
-      </c>
-      <c r="G36" t="s">
-        <v>108</v>
-      </c>
-      <c r="H36" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" t="s">
-        <v>103</v>
-      </c>
-      <c r="J36" t="s">
-        <v>34</v>
-      </c>
-      <c r="K36" t="s">
-        <v>107</v>
-      </c>
-      <c r="L36" t="s">
-        <v>34</v>
-      </c>
-      <c r="M36" t="s">
-        <v>102</v>
-      </c>
-      <c r="N36" t="s">
-        <v>34</v>
-      </c>
-      <c r="O36" t="s">
-        <v>99</v>
-      </c>
-      <c r="P36" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>